<commit_message>
updated files for database connection
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A56E4D-D203-4DF5-AA5C-2AC8B88FB497}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147330D5-28C0-4AE7-A1E3-1E27B3F560C2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="reportname" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>No of sheets</t>
   </si>
@@ -80,13 +80,44 @@
     <t>default</t>
   </si>
   <si>
-    <t>Hive</t>
-  </si>
-  <si>
     <t>Report Name</t>
   </si>
   <si>
-    <t>Policy</t>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>ACITGDPRWN01</t>
+  </si>
+  <si>
+    <t>gosales</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>Pass1234$</t>
+  </si>
+  <si>
+    <t>select [ORDER_DETAIL_CODE],[QUANTITY],[UNIT_SALE_PRICE]*[QUANTITY] as Revenue from  [gosales].[ORDER_DETAILS]
+ where Order_Detail_Code in('1000001',
+'1000002',
+'1000013',
+'1000014',
+'1000015',
+'1000016',
+'1000017') order by [ORDER_DETAIL_CODE]</t>
+  </si>
+  <si>
+    <t>Order Detail</t>
+  </si>
+  <si>
+    <t>Sql</t>
   </si>
 </sst>
 </file>
@@ -182,7 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -192,6 +223,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -475,7 +509,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84C207F-3242-4518-9FA6-FA7B72DC9CF9}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -484,12 +520,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -503,7 +539,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B4F340-CA6B-41DC-99D9-7C72B6307E66}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,7 +580,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -555,12 +591,52 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A7C5F5-C656-4893-8AC7-8D1AECB2B751}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>